<commit_message>
Update DR. IJAZ - CONVOCATION - STATUS.xlsx
</commit_message>
<xml_diff>
--- a/DR. IJAZ - CONVOCATION - STATUS.xlsx
+++ b/DR. IJAZ - CONVOCATION - STATUS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CONVOCATION OVERALL DATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\bashir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9CAC140-D748-40FC-A9E9-34B053A739DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9259E6BD-3003-4609-A61C-89C11B556D9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="845" firstSheet="7" activeTab="10" xr2:uid="{7196D735-60E2-402C-809A-8B8FA7337809}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="845" firstSheet="7" activeTab="10" xr2:uid="{7196D735-60E2-402C-809A-8B8FA7337809}"/>
   </bookViews>
   <sheets>
     <sheet name="1 DECEMBER 2023" sheetId="1" r:id="rId1"/>
@@ -1296,9 +1296,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1336,7 +1336,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1442,7 +1442,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1584,7 +1584,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1599,18 +1599,18 @@
       <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="35.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="4"/>
+    <col min="5" max="5" width="11.109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="35.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>73</v>
       </c>
@@ -1630,7 +1630,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -1710,7 +1710,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -1770,7 +1770,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -1810,7 +1810,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -1830,7 +1830,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -1890,7 +1890,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -1910,7 +1910,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -1930,7 +1930,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>16</v>
       </c>
@@ -1950,7 +1950,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>17</v>
       </c>
@@ -1970,7 +1970,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>18</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>20</v>
       </c>
@@ -2030,7 +2030,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -2050,7 +2050,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>22</v>
       </c>
@@ -2070,7 +2070,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>23</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>24</v>
       </c>
@@ -2110,7 +2110,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>25</v>
       </c>
@@ -2130,7 +2130,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>26</v>
       </c>
@@ -2171,16 +2171,16 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.140625" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" style="12" customWidth="1"/>
+    <col min="3" max="3" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>92</v>
       </c>
@@ -2191,14 +2191,14 @@
         <v>192</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18"/>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
       <c r="E2" s="19"/>
     </row>
-    <row r="3" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
         <v>193</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="11" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="11" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>1</v>
       </c>
@@ -2228,7 +2228,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>2</v>
       </c>
@@ -2245,7 +2245,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>3</v>
       </c>
@@ -2254,7 +2254,7 @@
       <c r="D6" s="17"/>
       <c r="E6" s="10"/>
     </row>
-    <row r="7" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>4</v>
       </c>
@@ -2263,7 +2263,7 @@
       <c r="D7" s="17"/>
       <c r="E7" s="10"/>
     </row>
-    <row r="8" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>5</v>
       </c>
@@ -2272,7 +2272,7 @@
       <c r="D8" s="17"/>
       <c r="E8" s="10"/>
     </row>
-    <row r="9" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>6</v>
       </c>
@@ -2281,7 +2281,7 @@
       <c r="D9" s="17"/>
       <c r="E9" s="10"/>
     </row>
-    <row r="10" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>7</v>
       </c>
@@ -2290,7 +2290,7 @@
       <c r="D10" s="17"/>
       <c r="E10" s="10"/>
     </row>
-    <row r="11" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>8</v>
       </c>
@@ -2299,7 +2299,7 @@
       <c r="D11" s="17"/>
       <c r="E11" s="10"/>
     </row>
-    <row r="12" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>9</v>
       </c>
@@ -2327,20 +2327,20 @@
   </sheetPr>
   <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A58" zoomScale="110" zoomScaleNormal="100" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="110" zoomScaleNormal="100" zoomScaleSheetLayoutView="110" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.140625" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" style="12" customWidth="1"/>
+    <col min="3" max="3" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>316</v>
       </c>
@@ -2351,14 +2351,14 @@
         <v>320</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18"/>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
       <c r="E2" s="19"/>
     </row>
-    <row r="3" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
         <v>317</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="11" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="11" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>1</v>
       </c>
@@ -2388,7 +2388,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>2</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>3</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>4</v>
       </c>
@@ -2439,7 +2439,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>5</v>
       </c>
@@ -2456,7 +2456,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>6</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>7</v>
       </c>
@@ -2490,7 +2490,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>8</v>
       </c>
@@ -2507,7 +2507,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>9</v>
       </c>
@@ -2524,7 +2524,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8">
         <v>10</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <v>11</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <v>12</v>
       </c>
@@ -2575,7 +2575,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>13</v>
       </c>
@@ -2592,7 +2592,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>14</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
         <v>15</v>
       </c>
@@ -2626,7 +2626,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <v>16</v>
       </c>
@@ -2643,7 +2643,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
         <v>17</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8">
         <v>18</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8">
         <v>19</v>
       </c>
@@ -2694,7 +2694,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8">
         <v>20</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8">
         <v>21</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8">
         <v>22</v>
       </c>
@@ -2745,7 +2745,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="8">
         <v>23</v>
       </c>
@@ -2762,7 +2762,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="8">
         <v>24</v>
       </c>
@@ -2779,7 +2779,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="8">
         <v>25</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="8">
         <v>26</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8">
         <v>27</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="8">
         <v>28</v>
       </c>
@@ -2847,7 +2847,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="8">
         <v>29</v>
       </c>
@@ -2864,7 +2864,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8">
         <v>30</v>
       </c>
@@ -2881,7 +2881,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8">
         <v>31</v>
       </c>
@@ -2898,7 +2898,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8">
         <v>32</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8">
         <v>33</v>
       </c>
@@ -2932,7 +2932,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="8">
         <v>34</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8">
         <v>35</v>
       </c>
@@ -2966,7 +2966,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="8">
         <v>36</v>
       </c>
@@ -2983,7 +2983,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="8">
         <v>37</v>
       </c>
@@ -3000,7 +3000,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="8">
         <v>38</v>
       </c>
@@ -3017,7 +3017,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="8">
         <v>39</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="8">
         <v>40</v>
       </c>
@@ -3051,7 +3051,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="8">
         <v>41</v>
       </c>
@@ -3068,7 +3068,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="8">
         <v>42</v>
       </c>
@@ -3085,7 +3085,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="8">
         <v>43</v>
       </c>
@@ -3102,7 +3102,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="8">
         <v>44</v>
       </c>
@@ -3119,7 +3119,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="48" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="8">
         <v>45</v>
       </c>
@@ -3136,7 +3136,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="8">
         <v>46</v>
       </c>
@@ -3153,7 +3153,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="8">
         <v>47</v>
       </c>
@@ -3170,7 +3170,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="8">
         <v>48</v>
       </c>
@@ -3187,7 +3187,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="8">
         <v>49</v>
       </c>
@@ -3204,7 +3204,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="8">
         <v>50</v>
       </c>
@@ -3221,7 +3221,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="8">
         <v>51</v>
       </c>
@@ -3238,7 +3238,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="55" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="8">
         <v>52</v>
       </c>
@@ -3255,7 +3255,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="8">
         <v>53</v>
       </c>
@@ -3272,7 +3272,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="57" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="8">
         <v>54</v>
       </c>
@@ -3289,7 +3289,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="58" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="8">
         <v>55</v>
       </c>
@@ -3306,7 +3306,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="8">
         <v>56</v>
       </c>
@@ -3323,7 +3323,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="60" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="8">
         <v>57</v>
       </c>
@@ -3351,7 +3351,7 @@
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.2" right="0.2" top="0" bottom="0.5" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="31" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="29" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3363,17 +3363,17 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.28515625" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.33203125" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="52.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>92</v>
       </c>
@@ -3383,7 +3383,7 @@
       <c r="E1" s="23"/>
       <c r="F1" s="23"/>
     </row>
-    <row r="2" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -3403,7 +3403,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -3423,7 +3423,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -3443,7 +3443,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -3463,7 +3463,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -3483,7 +3483,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="11" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="11" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -3523,7 +3523,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -3543,7 +3543,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -3563,7 +3563,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>10</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>11</v>
       </c>
@@ -3603,7 +3603,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8">
         <v>12</v>
       </c>
@@ -3623,7 +3623,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <v>13</v>
       </c>
@@ -3643,7 +3643,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <v>14</v>
       </c>
@@ -3663,7 +3663,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>15</v>
       </c>
@@ -3704,17 +3704,17 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.28515625" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.33203125" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="52.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>92</v>
       </c>
@@ -3726,7 +3726,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -3746,7 +3746,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -3766,7 +3766,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="11" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="11" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -3786,7 +3786,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -3806,7 +3806,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -3826,7 +3826,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -3846,7 +3846,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -3866,7 +3866,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -3886,7 +3886,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -3906,7 +3906,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>10</v>
       </c>
@@ -3926,7 +3926,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>11</v>
       </c>
@@ -3946,7 +3946,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8">
         <v>12</v>
       </c>
@@ -3987,16 +3987,16 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="44.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.140625" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" style="12" customWidth="1"/>
+    <col min="3" max="3" width="44.5546875" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>92</v>
       </c>
@@ -4007,14 +4007,14 @@
         <v>121</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18"/>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
       <c r="E2" s="19"/>
     </row>
-    <row r="3" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>122</v>
       </c>
@@ -4027,7 +4027,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>1</v>
       </c>
@@ -4044,7 +4044,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>2</v>
       </c>
@@ -4061,7 +4061,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="11" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="11" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>3</v>
       </c>
@@ -4078,7 +4078,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>4</v>
       </c>
@@ -4095,7 +4095,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>5</v>
       </c>
@@ -4112,7 +4112,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>6</v>
       </c>
@@ -4129,7 +4129,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>7</v>
       </c>
@@ -4146,7 +4146,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>8</v>
       </c>
@@ -4163,7 +4163,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>9</v>
       </c>
@@ -4180,7 +4180,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8">
         <v>10</v>
       </c>
@@ -4197,7 +4197,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <v>11</v>
       </c>
@@ -4237,16 +4237,16 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="44.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.140625" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" style="12" customWidth="1"/>
+    <col min="3" max="3" width="44.5546875" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>92</v>
       </c>
@@ -4257,14 +4257,14 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18"/>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
       <c r="E2" s="19"/>
     </row>
-    <row r="3" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>139</v>
       </c>
@@ -4277,7 +4277,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>1</v>
       </c>
@@ -4294,7 +4294,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>2</v>
       </c>
@@ -4311,7 +4311,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="11" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="11" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>3</v>
       </c>
@@ -4328,7 +4328,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>4</v>
       </c>
@@ -4345,7 +4345,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>5</v>
       </c>
@@ -4362,7 +4362,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>6</v>
       </c>
@@ -4379,7 +4379,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>7</v>
       </c>
@@ -4396,7 +4396,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>8</v>
       </c>
@@ -4413,7 +4413,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>9</v>
       </c>
@@ -4430,7 +4430,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8">
         <v>10</v>
       </c>
@@ -4447,7 +4447,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <v>11</v>
       </c>
@@ -4464,7 +4464,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <v>12</v>
       </c>
@@ -4481,7 +4481,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>13</v>
       </c>
@@ -4521,17 +4521,17 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="53.140625" customWidth="1"/>
+    <col min="3" max="3" width="28.109375" style="12" customWidth="1"/>
+    <col min="4" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>92</v>
       </c>
@@ -4543,7 +4543,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18"/>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
@@ -4551,7 +4551,7 @@
       <c r="E2" s="18"/>
       <c r="F2" s="19"/>
     </row>
-    <row r="3" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>157</v>
       </c>
@@ -4565,7 +4565,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>1</v>
       </c>
@@ -4585,7 +4585,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>2</v>
       </c>
@@ -4605,7 +4605,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>3</v>
       </c>
@@ -4625,7 +4625,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="11" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="11" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>4</v>
       </c>
@@ -4645,7 +4645,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>5</v>
       </c>
@@ -4665,7 +4665,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>6</v>
       </c>
@@ -4685,7 +4685,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>7</v>
       </c>
@@ -4705,7 +4705,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>8</v>
       </c>
@@ -4725,7 +4725,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>9</v>
       </c>
@@ -4745,7 +4745,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8">
         <v>10</v>
       </c>
@@ -4765,7 +4765,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <v>11</v>
       </c>
@@ -4785,7 +4785,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <v>12</v>
       </c>
@@ -4805,7 +4805,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>13</v>
       </c>
@@ -4825,7 +4825,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>14</v>
       </c>
@@ -4845,7 +4845,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
         <v>15</v>
       </c>
@@ -4888,17 +4888,17 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="53.140625" customWidth="1"/>
+    <col min="3" max="3" width="28.109375" style="12" customWidth="1"/>
+    <col min="4" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>92</v>
       </c>
@@ -4910,7 +4910,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18"/>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
@@ -4918,7 +4918,7 @@
       <c r="E2" s="18"/>
       <c r="F2" s="19"/>
     </row>
-    <row r="3" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>161</v>
       </c>
@@ -4932,7 +4932,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>1</v>
       </c>
@@ -4952,7 +4952,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>2</v>
       </c>
@@ -4972,7 +4972,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>3</v>
       </c>
@@ -4992,7 +4992,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="11" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="11" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>4</v>
       </c>
@@ -5012,7 +5012,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>5</v>
       </c>
@@ -5032,7 +5032,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>6</v>
       </c>
@@ -5052,7 +5052,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>7</v>
       </c>
@@ -5072,7 +5072,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>8</v>
       </c>
@@ -5092,7 +5092,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>9</v>
       </c>
@@ -5112,7 +5112,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8">
         <v>10</v>
       </c>
@@ -5132,7 +5132,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <v>11</v>
       </c>
@@ -5152,7 +5152,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <v>12</v>
       </c>
@@ -5198,17 +5198,17 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="53.140625" customWidth="1"/>
+    <col min="3" max="3" width="28.109375" style="12" customWidth="1"/>
+    <col min="4" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>92</v>
       </c>
@@ -5220,7 +5220,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18"/>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
@@ -5228,7 +5228,7 @@
       <c r="E2" s="18"/>
       <c r="F2" s="19"/>
     </row>
-    <row r="3" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
         <v>185</v>
       </c>
@@ -5242,7 +5242,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="11" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="11" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>1</v>
       </c>
@@ -5262,7 +5262,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>2</v>
       </c>
@@ -5282,7 +5282,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>3</v>
       </c>
@@ -5302,7 +5302,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>4</v>
       </c>
@@ -5322,7 +5322,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>5</v>
       </c>
@@ -5342,7 +5342,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>6</v>
       </c>
@@ -5362,7 +5362,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>7</v>
       </c>
@@ -5382,7 +5382,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>8</v>
       </c>
@@ -5428,17 +5428,17 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="53.140625" customWidth="1"/>
+    <col min="3" max="3" width="28.109375" style="12" customWidth="1"/>
+    <col min="4" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>92</v>
       </c>
@@ -5450,7 +5450,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18"/>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
@@ -5458,7 +5458,7 @@
       <c r="E2" s="18"/>
       <c r="F2" s="19"/>
     </row>
-    <row r="3" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
         <v>190</v>
       </c>
@@ -5472,7 +5472,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="11" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="11" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>1</v>
       </c>
@@ -5492,7 +5492,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>2</v>
       </c>

</xml_diff>